<commit_message>
Deploying to gh-pages from  @ 03fb76b9ac146585df05395f980ae353fb99e762 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.1.xlsx
+++ b/en/downloads/data-excel/1.2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>Наименование показателей</t>
   </si>
@@ -178,30 +178,6 @@
     <t>Working age population (women 16-57 years old, men 16-62 years old)</t>
   </si>
   <si>
-    <t>Пол</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Жыныс</t>
-  </si>
-  <si>
-    <t>Возраст</t>
-  </si>
-  <si>
-    <t>Жаш курагы</t>
-  </si>
-  <si>
-    <t>Аймак</t>
-  </si>
-  <si>
-    <t>Область</t>
-  </si>
-  <si>
-    <t>Territory</t>
-  </si>
-  <si>
     <t>Население старше трудоспособного возраста (женщины 58 лет и старше, мужчины 63 лет и старше)</t>
   </si>
   <si>
@@ -212,6 +188,60 @@
   </si>
   <si>
     <t>Эмгекке жарактуу жаштан жогорку калктын саны (58 жана андан жогорку жаштагы аялдар, 63 жана андан жогорку жаштагы эркектер)</t>
+  </si>
+  <si>
+    <t>Аймактар боюнча</t>
+  </si>
+  <si>
+    <t>По территории</t>
+  </si>
+  <si>
+    <t>By territory</t>
+  </si>
+  <si>
+    <t>Жаш курак топтор боюнча</t>
+  </si>
+  <si>
+    <t>По возрастным группам</t>
+  </si>
+  <si>
+    <t>By age group</t>
+  </si>
+  <si>
+    <t>Жынысы боюнча</t>
+  </si>
+  <si>
+    <t>По полу</t>
+  </si>
+  <si>
+    <t>By sex</t>
+  </si>
+  <si>
+    <t>Жерлери</t>
+  </si>
+  <si>
+    <t>Местность</t>
+  </si>
+  <si>
+    <t>Urbanisation</t>
+  </si>
+  <si>
+    <t>Шаар</t>
+  </si>
+  <si>
+    <t>Городские поселения</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Айыл</t>
+  </si>
+  <si>
+    <t>Сельская местность</t>
+  </si>
+  <si>
+    <t>Village</t>
   </si>
 </sst>
 </file>
@@ -388,7 +418,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,7 +506,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -805,7 +834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -888,6 +917,9 @@
       <c r="P4" s="15">
         <v>2019</v>
       </c>
+      <c r="Q4" s="15">
+        <v>2020</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
@@ -938,16 +970,19 @@
       <c r="P5" s="25">
         <v>20.124198474961176</v>
       </c>
+      <c r="Q5" s="25">
+        <v>25.3</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>55</v>
+      <c r="A6" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -962,6 +997,7 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1012,7 +1048,9 @@
       <c r="P7" s="16">
         <v>20.078519398883305</v>
       </c>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="16">
+        <v>25.3</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
     </row>
@@ -1065,18 +1103,22 @@
       <c r="P8" s="16">
         <v>20.175708173042036</v>
       </c>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="16">
+        <v>25.3</v>
+      </c>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="36"/>
+      <c r="A9" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>69</v>
+      </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -1090,169 +1132,132 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="7"/>
+      <c r="Q9" s="16"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="16">
-        <v>45.2</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16">
+        <v>23.6</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="16">
-        <v>37.9</v>
+        <v>26.9</v>
       </c>
       <c r="L10" s="16">
-        <v>40.5</v>
+        <v>29.3</v>
       </c>
       <c r="M10" s="16">
-        <v>31.5</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="N10" s="16">
-        <v>32</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="O10" s="16">
-        <v>28.3</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="P10" s="16">
-        <v>25.7</v>
-      </c>
+        <v>14.7</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>18.3</v>
+      </c>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="16">
-        <v>35.6</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16">
+        <v>39.5</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="16">
-        <v>28.5</v>
+        <v>32.6</v>
       </c>
       <c r="L11" s="16">
+        <v>33.6</v>
+      </c>
+      <c r="M11" s="16">
         <v>29</v>
       </c>
-      <c r="M11" s="16">
-        <v>23</v>
-      </c>
       <c r="N11" s="16">
-        <v>22.9</v>
+        <v>28.4</v>
       </c>
       <c r="O11" s="16">
-        <v>20.9</v>
+        <v>23.7</v>
       </c>
       <c r="P11" s="16">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="16">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="K12" s="16">
-        <v>27</v>
-      </c>
-      <c r="L12" s="16">
-        <v>27.9</v>
-      </c>
-      <c r="M12" s="16">
-        <v>21.8</v>
-      </c>
-      <c r="N12" s="16">
-        <v>22</v>
-      </c>
-      <c r="O12" s="16">
-        <v>19.3</v>
-      </c>
-      <c r="P12" s="16">
-        <v>17.117237487541317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="3" t="s">
+        <v>23.2</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>29.3</v>
+      </c>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C12" s="35" t="s">
         <v>63</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>46</v>
@@ -1273,570 +1278,594 @@
         <v>46</v>
       </c>
       <c r="J13" s="16">
+        <v>45.2</v>
+      </c>
+      <c r="K13" s="16">
+        <v>37.9</v>
+      </c>
+      <c r="L13" s="16">
+        <v>40.5</v>
+      </c>
+      <c r="M13" s="16">
+        <v>31.5</v>
+      </c>
+      <c r="N13" s="16">
+        <v>32</v>
+      </c>
+      <c r="O13" s="16">
+        <v>28.3</v>
+      </c>
+      <c r="P13" s="16">
+        <v>25.7</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="16">
+        <v>35.6</v>
+      </c>
+      <c r="K14" s="16">
+        <v>28.5</v>
+      </c>
+      <c r="L14" s="16">
+        <v>29</v>
+      </c>
+      <c r="M14" s="16">
+        <v>23</v>
+      </c>
+      <c r="N14" s="16">
+        <v>22.9</v>
+      </c>
+      <c r="O14" s="16">
+        <v>20.9</v>
+      </c>
+      <c r="P14" s="16">
+        <v>16.2</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="16">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K15" s="16">
+        <v>27</v>
+      </c>
+      <c r="L15" s="16">
+        <v>27.9</v>
+      </c>
+      <c r="M15" s="16">
+        <v>21.8</v>
+      </c>
+      <c r="N15" s="16">
+        <v>22</v>
+      </c>
+      <c r="O15" s="16">
+        <v>19.3</v>
+      </c>
+      <c r="P15" s="16">
+        <v>17.117237487541317</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="16">
         <v>25.2</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K16" s="16">
         <v>21.3</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L16" s="16">
         <v>21.8</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M16" s="16">
         <v>19.899999999999999</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N16" s="16">
         <v>18.899999999999999</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O16" s="16">
         <v>14.8</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P16" s="16">
         <v>13.285423782570058</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="Q16" s="16">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="C17" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D18" s="16">
         <v>40.402479889759874</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E18" s="16">
         <v>20.741559677258106</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F18" s="16">
         <v>31.472533233133365</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G18" s="16">
         <v>33.595651944803727</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H18" s="16">
         <v>35.637925280764073</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I18" s="16">
         <v>34.235279979054241</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J18" s="16">
         <v>53.855810041406322</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K18" s="16">
         <v>40.719691825525814</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L18" s="16">
         <v>41.156482988237698</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M18" s="16">
         <v>37.049867142684406</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N18" s="16">
         <v>40.518930421912231</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O18" s="16">
         <v>33.773947202914634</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P18" s="16">
         <v>32.60027766870374</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="16">
-        <v>41.298197061272944</v>
-      </c>
-      <c r="E16" s="16">
-        <v>22.400606661789254</v>
-      </c>
-      <c r="F16" s="16">
-        <v>31.273920861021736</v>
-      </c>
-      <c r="G16" s="16">
-        <v>31.928277981030423</v>
-      </c>
-      <c r="H16" s="16">
-        <v>34.181401408145312</v>
-      </c>
-      <c r="I16" s="16">
-        <v>34.639723309128705</v>
-      </c>
-      <c r="J16" s="16">
-        <v>53.627066611694964</v>
-      </c>
-      <c r="K16" s="16">
-        <v>39.011011201209385</v>
-      </c>
-      <c r="L16" s="16">
-        <v>40.926453617457369</v>
-      </c>
-      <c r="M16" s="16">
-        <v>36.116546796954033</v>
-      </c>
-      <c r="N16" s="16">
-        <v>39.604539591896497</v>
-      </c>
-      <c r="O16" s="16">
-        <v>33.671053924880781</v>
-      </c>
-      <c r="P16" s="16">
-        <v>32.424873967888452</v>
-      </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="16">
-        <v>39.381263817790511</v>
-      </c>
-      <c r="E17" s="16">
-        <v>18.757342571657283</v>
-      </c>
-      <c r="F17" s="16">
-        <v>31.703884845676683</v>
-      </c>
-      <c r="G17" s="16">
-        <v>35.55793402205002</v>
-      </c>
-      <c r="H17" s="16">
-        <v>37.347648282219502</v>
-      </c>
-      <c r="I17" s="16">
-        <v>33.764476225800678</v>
-      </c>
-      <c r="J17" s="16">
-        <v>54.08783910774202</v>
-      </c>
-      <c r="K17" s="16">
-        <v>42.448702330320252</v>
-      </c>
-      <c r="L17" s="16">
-        <v>41.395881762864036</v>
-      </c>
-      <c r="M17" s="16">
-        <v>38.033368857397804</v>
-      </c>
-      <c r="N17" s="16">
-        <v>41.521176404727939</v>
-      </c>
-      <c r="O17" s="16">
-        <v>33.888978930781725</v>
-      </c>
-      <c r="P17" s="16">
-        <v>32.794370380144969</v>
-      </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="16">
-        <v>53.037853145464332</v>
-      </c>
-      <c r="E18" s="16">
-        <v>40.086270531670472</v>
-      </c>
-      <c r="F18" s="16">
-        <v>36.873144430974918</v>
-      </c>
-      <c r="G18" s="16">
-        <v>44.705496370584875</v>
-      </c>
-      <c r="H18" s="16">
-        <v>45.290428057708084</v>
-      </c>
-      <c r="I18" s="16">
-        <v>55.657830690086428</v>
-      </c>
-      <c r="J18" s="16">
-        <v>46.41253835816282</v>
-      </c>
-      <c r="K18" s="16">
-        <v>46.435379481648589</v>
-      </c>
-      <c r="L18" s="16">
-        <v>45.092334897269765</v>
-      </c>
-      <c r="M18" s="16">
-        <v>32.247345241286098</v>
-      </c>
-      <c r="N18" s="16">
-        <v>32.580650410531696</v>
-      </c>
-      <c r="O18" s="16">
-        <v>32.215180398381278</v>
-      </c>
-      <c r="P18" s="16">
-        <v>26.949229229116593</v>
-      </c>
-      <c r="Q18" s="31"/>
+      <c r="Q18" s="16">
+        <v>34.700000000000003</v>
+      </c>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="16">
-        <v>51.581913300980112</v>
+        <v>41.298197061272944</v>
       </c>
       <c r="E19" s="16">
-        <v>37.898730956037639</v>
+        <v>22.400606661789254</v>
       </c>
       <c r="F19" s="16">
-        <v>33.475026855982897</v>
+        <v>31.273920861021736</v>
       </c>
       <c r="G19" s="16">
-        <v>43.666947672535464</v>
+        <v>31.928277981030423</v>
       </c>
       <c r="H19" s="16">
-        <v>43.691713616679245</v>
+        <v>34.181401408145312</v>
       </c>
       <c r="I19" s="16">
-        <v>55.271782333465687</v>
+        <v>34.639723309128705</v>
       </c>
       <c r="J19" s="16">
-        <v>47.356835988795638</v>
+        <v>53.627066611694964</v>
       </c>
       <c r="K19" s="16">
-        <v>47.010504519675102</v>
+        <v>39.011011201209385</v>
       </c>
       <c r="L19" s="16">
-        <v>45.246248393795341</v>
+        <v>40.926453617457369</v>
       </c>
       <c r="M19" s="16">
-        <v>33.070935081614579</v>
+        <v>36.116546796954033</v>
       </c>
       <c r="N19" s="16">
-        <v>33.991287702261047</v>
+        <v>39.604539591896497</v>
       </c>
       <c r="O19" s="16">
-        <v>33.427506155728132</v>
+        <v>33.671053924880781</v>
       </c>
       <c r="P19" s="16">
-        <v>27.837054029315262</v>
-      </c>
-      <c r="Q19" s="31"/>
+        <v>32.424873967888452</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>34.299999999999997</v>
+      </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="16">
+        <v>39.381263817790511</v>
+      </c>
+      <c r="E20" s="16">
+        <v>18.757342571657283</v>
+      </c>
+      <c r="F20" s="16">
+        <v>31.703884845676683</v>
+      </c>
+      <c r="G20" s="16">
+        <v>35.55793402205002</v>
+      </c>
+      <c r="H20" s="16">
+        <v>37.347648282219502</v>
+      </c>
+      <c r="I20" s="16">
+        <v>33.764476225800678</v>
+      </c>
+      <c r="J20" s="16">
+        <v>54.08783910774202</v>
+      </c>
+      <c r="K20" s="16">
+        <v>42.448702330320252</v>
+      </c>
+      <c r="L20" s="16">
+        <v>41.395881762864036</v>
+      </c>
+      <c r="M20" s="16">
+        <v>38.033368857397804</v>
+      </c>
+      <c r="N20" s="16">
+        <v>41.521176404727939</v>
+      </c>
+      <c r="O20" s="16">
+        <v>33.888978930781725</v>
+      </c>
+      <c r="P20" s="16">
+        <v>32.794370380144969</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>35.1</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="16">
+        <v>53.037853145464332</v>
+      </c>
+      <c r="E21" s="16">
+        <v>40.086270531670472</v>
+      </c>
+      <c r="F21" s="16">
+        <v>36.873144430974918</v>
+      </c>
+      <c r="G21" s="16">
+        <v>44.705496370584875</v>
+      </c>
+      <c r="H21" s="16">
+        <v>45.290428057708084</v>
+      </c>
+      <c r="I21" s="16">
+        <v>55.657830690086428</v>
+      </c>
+      <c r="J21" s="16">
+        <v>46.41253835816282</v>
+      </c>
+      <c r="K21" s="16">
+        <v>46.435379481648589</v>
+      </c>
+      <c r="L21" s="16">
+        <v>45.092334897269765</v>
+      </c>
+      <c r="M21" s="16">
+        <v>32.247345241286098</v>
+      </c>
+      <c r="N21" s="16">
+        <v>32.580650410531696</v>
+      </c>
+      <c r="O21" s="16">
+        <v>32.215180398381278</v>
+      </c>
+      <c r="P21" s="16">
+        <v>26.949229229116593</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="16">
+        <v>51.581913300980112</v>
+      </c>
+      <c r="E22" s="16">
+        <v>37.898730956037639</v>
+      </c>
+      <c r="F22" s="16">
+        <v>33.475026855982897</v>
+      </c>
+      <c r="G22" s="16">
+        <v>43.666947672535464</v>
+      </c>
+      <c r="H22" s="16">
+        <v>43.691713616679245</v>
+      </c>
+      <c r="I22" s="16">
+        <v>55.271782333465687</v>
+      </c>
+      <c r="J22" s="16">
+        <v>47.356835988795638</v>
+      </c>
+      <c r="K22" s="16">
+        <v>47.010504519675102</v>
+      </c>
+      <c r="L22" s="16">
+        <v>45.246248393795341</v>
+      </c>
+      <c r="M22" s="16">
+        <v>33.070935081614579</v>
+      </c>
+      <c r="N22" s="16">
+        <v>33.991287702261047</v>
+      </c>
+      <c r="O22" s="16">
+        <v>33.427506155728132</v>
+      </c>
+      <c r="P22" s="16">
+        <v>27.837054029315262</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>39</v>
+      </c>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="16">
         <v>54.569085687052358</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E23" s="16">
         <v>42.427936426011655</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F23" s="16">
         <v>40.528056096234025</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G23" s="16">
         <v>45.762935658295987</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H23" s="16">
         <v>46.925945902420438</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I23" s="16">
         <v>56.050612838025486</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J23" s="16">
         <v>45.459523948653484</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K23" s="16">
         <v>45.842337649953734</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L23" s="16">
         <v>44.933484159094526</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M23" s="16">
         <v>31.382457734244912</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N23" s="16">
         <v>31.110381241015197</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O23" s="16">
         <v>30.92489536681844</v>
       </c>
-      <c r="P20" s="16">
+      <c r="P23" s="16">
         <v>26.006375104165304</v>
       </c>
-      <c r="Q20" s="31"/>
-    </row>
-    <row r="21" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="Q23" s="16">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B24" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C24" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D24" s="16">
         <v>38.587156397141321</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E24" s="16">
         <v>52.243735659060569</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F24" s="16">
         <v>46.090373783194451</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G24" s="16">
         <v>38.013539204566712</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H24" s="16">
         <v>29.522754727724266</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I24" s="16">
         <v>28.137635133798742</v>
       </c>
-      <c r="J21" s="16">
+      <c r="J24" s="16">
         <v>39.477989961494835</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K24" s="16">
         <v>26.014325183400164</v>
       </c>
-      <c r="L21" s="16">
+      <c r="L24" s="16">
         <v>28.892638246691408</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M24" s="16">
         <v>24.74455342190311</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N24" s="16">
         <v>24.170328861189912</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O24" s="16">
         <v>21.529510496448221</v>
       </c>
-      <c r="P21" s="16">
+      <c r="P24" s="16">
         <v>24.449709453745115</v>
       </c>
-      <c r="Q21" s="31"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="16">
-        <v>38.684593590774618</v>
-      </c>
-      <c r="E22" s="16">
-        <v>52.152947022826481</v>
-      </c>
-      <c r="F22" s="16">
-        <v>47.889059425246316</v>
-      </c>
-      <c r="G22" s="16">
-        <v>36.910698798507255</v>
-      </c>
-      <c r="H22" s="16">
-        <v>31.115103240448146</v>
-      </c>
-      <c r="I22" s="16">
-        <v>28.242617789669175</v>
-      </c>
-      <c r="J22" s="16">
-        <v>40.426190005675039</v>
-      </c>
-      <c r="K22" s="16">
-        <v>26.3548130266553</v>
-      </c>
-      <c r="L22" s="16">
-        <v>29.078560303070596</v>
-      </c>
-      <c r="M22" s="16">
-        <v>24.749641705183127</v>
-      </c>
-      <c r="N22" s="16">
-        <v>24.266813149633116</v>
-      </c>
-      <c r="O22" s="16">
-        <v>21.495640575964732</v>
-      </c>
-      <c r="P22" s="16">
-        <v>25.261407984004691</v>
-      </c>
-      <c r="Q22" s="31"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="16">
-        <v>38.498842893622495</v>
-      </c>
-      <c r="E23" s="16">
-        <v>52.320360206669946</v>
-      </c>
-      <c r="F23" s="16">
-        <v>44.512909658620337</v>
-      </c>
-      <c r="G23" s="16">
-        <v>39.00628927384588</v>
-      </c>
-      <c r="H23" s="16">
-        <v>28.11224725260351</v>
-      </c>
-      <c r="I23" s="16">
-        <v>28.021324105956992</v>
-      </c>
-      <c r="J23" s="16">
-        <v>38.474804276820919</v>
-      </c>
-      <c r="K23" s="16">
-        <v>25.663078513514154</v>
-      </c>
-      <c r="L23" s="16">
-        <v>28.701454292915692</v>
-      </c>
-      <c r="M23" s="16">
-        <v>24.739204448529353</v>
-      </c>
-      <c r="N23" s="16">
-        <v>24.067406584555748</v>
-      </c>
-      <c r="O23" s="16">
-        <v>21.566132496570411</v>
-      </c>
-      <c r="P23" s="16">
-        <v>23.571244210416801</v>
-      </c>
-      <c r="Q23" s="31"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="16">
-        <v>45.182678649814314</v>
-      </c>
-      <c r="E24" s="16">
-        <v>42.730283811653365</v>
-      </c>
-      <c r="F24" s="16">
-        <v>44.117919691307137</v>
-      </c>
-      <c r="G24" s="16">
-        <v>53.531335146815451</v>
-      </c>
-      <c r="H24" s="16">
-        <v>49.925097790099393</v>
-      </c>
-      <c r="I24" s="16">
-        <v>39.932299240936274</v>
-      </c>
-      <c r="J24" s="16">
-        <v>43.754395294404411</v>
-      </c>
-      <c r="K24" s="16">
-        <v>30.560926744429675</v>
-      </c>
-      <c r="L24" s="16">
-        <v>38.007028694030566</v>
-      </c>
-      <c r="M24" s="16">
-        <v>37.79821150847107</v>
-      </c>
-      <c r="N24" s="16">
-        <v>29.21833950434447</v>
-      </c>
-      <c r="O24" s="16">
-        <v>30.596327932893466</v>
-      </c>
-      <c r="P24" s="16">
-        <v>28.138697667467131</v>
-      </c>
-      <c r="Q24" s="31"/>
+      <c r="Q24" s="16">
+        <v>27.9</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1849,45 +1878,47 @@
         <v>33</v>
       </c>
       <c r="D25" s="16">
-        <v>46.868158500298755</v>
+        <v>38.684593590774618</v>
       </c>
       <c r="E25" s="16">
-        <v>42.698866213804251</v>
+        <v>52.152947022826481</v>
       </c>
       <c r="F25" s="16">
-        <v>44.838863302106681</v>
+        <v>47.889059425246316</v>
       </c>
       <c r="G25" s="16">
-        <v>53.397508505190693</v>
+        <v>36.910698798507255</v>
       </c>
       <c r="H25" s="16">
-        <v>48.269823904649712</v>
+        <v>31.115103240448146</v>
       </c>
       <c r="I25" s="16">
-        <v>37.664069415042029</v>
+        <v>28.242617789669175</v>
       </c>
       <c r="J25" s="16">
-        <v>44.781414591166033</v>
+        <v>40.426190005675039</v>
       </c>
       <c r="K25" s="16">
-        <v>32.369300618626895</v>
+        <v>26.3548130266553</v>
       </c>
       <c r="L25" s="16">
-        <v>39.504743553298205</v>
+        <v>29.078560303070596</v>
       </c>
       <c r="M25" s="16">
-        <v>39.601891368837386</v>
+        <v>24.749641705183127</v>
       </c>
       <c r="N25" s="16">
-        <v>31.189138362275092</v>
+        <v>24.266813149633116</v>
       </c>
       <c r="O25" s="16">
-        <v>31.594899662350688</v>
+        <v>21.495640575964732</v>
       </c>
       <c r="P25" s="16">
-        <v>28.978045168904039</v>
-      </c>
-      <c r="Q25" s="31"/>
+        <v>25.261407984004691</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1900,455 +1931,473 @@
         <v>4</v>
       </c>
       <c r="D26" s="16">
-        <v>43.678264522994652</v>
+        <v>38.498842893622495</v>
       </c>
       <c r="E26" s="16">
-        <v>42.757724565987253</v>
+        <v>52.320360206669946</v>
       </c>
       <c r="F26" s="16">
-        <v>43.49630815436538</v>
+        <v>44.512909658620337</v>
       </c>
       <c r="G26" s="16">
-        <v>53.676667578832138</v>
+        <v>39.00628927384588</v>
       </c>
       <c r="H26" s="16">
-        <v>51.7285367396859</v>
+        <v>28.11224725260351</v>
       </c>
       <c r="I26" s="16">
-        <v>42.395906143747297</v>
+        <v>28.021324105956992</v>
       </c>
       <c r="J26" s="16">
-        <v>42.671843342389494</v>
+        <v>38.474804276820919</v>
       </c>
       <c r="K26" s="16">
-        <v>28.643083188639221</v>
+        <v>25.663078513514154</v>
       </c>
       <c r="L26" s="16">
-        <v>36.407724820754808</v>
+        <v>28.701454292915692</v>
       </c>
       <c r="M26" s="16">
-        <v>35.859946286618936</v>
+        <v>24.739204448529353</v>
       </c>
       <c r="N26" s="16">
-        <v>27.069804008596218</v>
+        <v>24.067406584555748</v>
       </c>
       <c r="O26" s="16">
-        <v>29.460632166824883</v>
+        <v>21.566132496570411</v>
       </c>
       <c r="P26" s="16">
-        <v>27.215175085071412</v>
-      </c>
-      <c r="Q26" s="31"/>
+        <v>23.571244210416801</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D27" s="16">
-        <v>46.591609930340859</v>
+        <v>45.182678649814314</v>
       </c>
       <c r="E27" s="16">
-        <v>37.452826077173327</v>
+        <v>42.730283811653365</v>
       </c>
       <c r="F27" s="16">
-        <v>38.292035961047127</v>
+        <v>44.117919691307137</v>
       </c>
       <c r="G27" s="16">
-        <v>41.897117973076092</v>
+        <v>53.531335146815451</v>
       </c>
       <c r="H27" s="16">
-        <v>44.680774328796652</v>
+        <v>49.925097790099393</v>
       </c>
       <c r="I27" s="16">
-        <v>51.433697589627926</v>
+        <v>39.932299240936274</v>
       </c>
       <c r="J27" s="16">
-        <v>43.409368736792423</v>
+        <v>43.754395294404411</v>
       </c>
       <c r="K27" s="16">
-        <v>31.740140413309955</v>
+        <v>30.560926744429675</v>
       </c>
       <c r="L27" s="16">
-        <v>28.94451088455056</v>
+        <v>38.007028694030566</v>
       </c>
       <c r="M27" s="16">
-        <v>22.024662785484026</v>
+        <v>37.79821150847107</v>
       </c>
       <c r="N27" s="16">
-        <v>14.267617212396773</v>
+        <v>29.21833950434447</v>
       </c>
       <c r="O27" s="16">
-        <v>14.778619534247351</v>
+        <v>30.596327932893466</v>
       </c>
       <c r="P27" s="16">
-        <v>14.029577911075274</v>
-      </c>
-      <c r="Q27" s="31"/>
+        <v>28.138697667467131</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>36.799999999999997</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="16">
-        <v>48.708185613648588</v>
+        <v>46.868158500298755</v>
       </c>
       <c r="E28" s="16">
-        <v>37.931553813927593</v>
+        <v>42.698866213804251</v>
       </c>
       <c r="F28" s="16">
-        <v>38.33463619585136</v>
+        <v>44.838863302106681</v>
       </c>
       <c r="G28" s="16">
-        <v>40.639754074948065</v>
+        <v>53.397508505190693</v>
       </c>
       <c r="H28" s="16">
-        <v>44.16969494757889</v>
+        <v>48.269823904649712</v>
       </c>
       <c r="I28" s="16">
-        <v>50.553915555212974</v>
+        <v>37.664069415042029</v>
       </c>
       <c r="J28" s="16">
-        <v>42.660818605433128</v>
+        <v>44.781414591166033</v>
       </c>
       <c r="K28" s="16">
-        <v>30.494416878480461</v>
+        <v>32.369300618626895</v>
       </c>
       <c r="L28" s="16">
-        <v>28.438702897823607</v>
+        <v>39.504743553298205</v>
       </c>
       <c r="M28" s="16">
-        <v>21.810871896719039</v>
+        <v>39.601891368837386</v>
       </c>
       <c r="N28" s="16">
-        <v>12.948414919324932</v>
+        <v>31.189138362275092</v>
       </c>
       <c r="O28" s="16">
-        <v>15.256250012211552</v>
+        <v>31.594899662350688</v>
       </c>
       <c r="P28" s="16">
-        <v>14.136273808213584</v>
-      </c>
-      <c r="Q28" s="31"/>
+        <v>28.978045168904039</v>
+      </c>
+      <c r="Q28" s="16">
+        <v>37.6</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="16">
-        <v>44.295394408336584</v>
+        <v>43.678264522994652</v>
       </c>
       <c r="E29" s="16">
-        <v>36.913060085846247</v>
+        <v>42.757724565987253</v>
       </c>
       <c r="F29" s="16">
-        <v>38.245331717166891</v>
+        <v>43.49630815436538</v>
       </c>
       <c r="G29" s="16">
-        <v>43.246261432263722</v>
+        <v>53.676667578832138</v>
       </c>
       <c r="H29" s="16">
-        <v>45.2407499534715</v>
+        <v>51.7285367396859</v>
       </c>
       <c r="I29" s="16">
-        <v>52.418829921890676</v>
+        <v>42.395906143747297</v>
       </c>
       <c r="J29" s="16">
-        <v>44.228326041983919</v>
+        <v>42.671843342389494</v>
       </c>
       <c r="K29" s="16">
-        <v>33.102942270087709</v>
+        <v>28.643083188639221</v>
       </c>
       <c r="L29" s="16">
-        <v>29.489510141633829</v>
+        <v>36.407724820754808</v>
       </c>
       <c r="M29" s="16">
-        <v>22.264452734141326</v>
+        <v>35.859946286618936</v>
       </c>
       <c r="N29" s="16">
-        <v>15.723494620754009</v>
+        <v>27.069804008596218</v>
       </c>
       <c r="O29" s="16">
-        <v>14.253421863029283</v>
+        <v>29.460632166824883</v>
       </c>
       <c r="P29" s="16">
-        <v>13.910068203555255</v>
-      </c>
-      <c r="Q29" s="31"/>
+        <v>27.215175085071412</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>35.9</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30" s="16">
-        <v>35.25905281064211</v>
+        <v>46.591609930340859</v>
       </c>
       <c r="E30" s="16">
-        <v>42.972123081253251</v>
+        <v>37.452826077173327</v>
       </c>
       <c r="F30" s="16">
-        <v>33.003964492164805</v>
+        <v>38.292035961047127</v>
       </c>
       <c r="G30" s="16">
-        <v>42.338833276680255</v>
+        <v>41.897117973076092</v>
       </c>
       <c r="H30" s="16">
-        <v>50.172706455002995</v>
+        <v>44.680774328796652</v>
       </c>
       <c r="I30" s="16">
-        <v>39.574780355782721</v>
+        <v>51.433697589627926</v>
       </c>
       <c r="J30" s="16">
-        <v>23.057182049490603</v>
+        <v>43.409368736792423</v>
       </c>
       <c r="K30" s="16">
-        <v>19.048344075891784</v>
+        <v>31.740140413309955</v>
       </c>
       <c r="L30" s="16">
-        <v>21.481514210162892</v>
+        <v>28.94451088455056</v>
       </c>
       <c r="M30" s="16">
-        <v>18.115850908998514</v>
+        <v>22.024662785484026</v>
       </c>
       <c r="N30" s="16">
-        <v>20.679702753300546</v>
+        <v>14.267617212396773</v>
       </c>
       <c r="O30" s="16">
-        <v>22.085933924873434</v>
+        <v>14.778619534247351</v>
       </c>
       <c r="P30" s="16">
-        <v>13.290366478193151</v>
-      </c>
-      <c r="Q30" s="31"/>
+        <v>14.029577911075274</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>18.8</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="16">
-        <v>35.524400738676341</v>
+        <v>48.708185613648588</v>
       </c>
       <c r="E31" s="16">
-        <v>45.403420335985643</v>
+        <v>37.931553813927593</v>
       </c>
       <c r="F31" s="16">
-        <v>35.67372171666905</v>
+        <v>38.33463619585136</v>
       </c>
       <c r="G31" s="16">
-        <v>44.324841323157756</v>
+        <v>40.639754074948065</v>
       </c>
       <c r="H31" s="16">
-        <v>51.365667230180513</v>
+        <v>44.16969494757889</v>
       </c>
       <c r="I31" s="16">
-        <v>42.155403417412046</v>
+        <v>50.553915555212974</v>
       </c>
       <c r="J31" s="16">
-        <v>23.320678028402405</v>
+        <v>42.660818605433128</v>
       </c>
       <c r="K31" s="16">
-        <v>19.717988374234295</v>
+        <v>30.494416878480461</v>
       </c>
       <c r="L31" s="16">
-        <v>22.565254965961532</v>
+        <v>28.438702897823607</v>
       </c>
       <c r="M31" s="16">
-        <v>19.131642435267874</v>
+        <v>21.810871896719039</v>
       </c>
       <c r="N31" s="16">
-        <v>21.405379816313594</v>
+        <v>12.948414919324932</v>
       </c>
       <c r="O31" s="16">
-        <v>23.802663209890316</v>
+        <v>15.256250012211552</v>
       </c>
       <c r="P31" s="16">
-        <v>13.968630674154097</v>
-      </c>
-      <c r="Q31" s="31"/>
+        <v>14.136273808213584</v>
+      </c>
+      <c r="Q31" s="16">
+        <v>18.899999999999999</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="16">
-        <v>34.937966325921565</v>
+        <v>44.295394408336584</v>
       </c>
       <c r="E32" s="16">
-        <v>40.025342396149952</v>
+        <v>36.913060085846247</v>
       </c>
       <c r="F32" s="16">
-        <v>29.757564599462217</v>
+        <v>38.245331717166891</v>
       </c>
       <c r="G32" s="16">
-        <v>40.090317720015314</v>
+        <v>43.246261432263722</v>
       </c>
       <c r="H32" s="16">
-        <v>48.834976975707399</v>
+        <v>45.2407499534715</v>
       </c>
       <c r="I32" s="16">
-        <v>36.737399067049523</v>
+        <v>52.418829921890676</v>
       </c>
       <c r="J32" s="16">
-        <v>22.797195558030481</v>
+        <v>44.228326041983919</v>
       </c>
       <c r="K32" s="16">
-        <v>18.388950301669212</v>
+        <v>33.102942270087709</v>
       </c>
       <c r="L32" s="16">
-        <v>20.402520679941826</v>
+        <v>29.489510141633829</v>
       </c>
       <c r="M32" s="16">
-        <v>17.094741091820271</v>
+        <v>22.264452734141326</v>
       </c>
       <c r="N32" s="16">
-        <v>19.940922159102712</v>
+        <v>15.723494620754009</v>
       </c>
       <c r="O32" s="16">
-        <v>20.340711553536092</v>
+        <v>14.253421863029283</v>
       </c>
       <c r="P32" s="16">
-        <v>12.593673786232706</v>
-      </c>
-      <c r="Q32" s="31"/>
+        <v>13.910068203555255</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D33" s="16">
-        <v>14.980993583120011</v>
+        <v>35.25905281064211</v>
       </c>
       <c r="E33" s="16">
-        <v>15.782630902499408</v>
+        <v>42.972123081253251</v>
       </c>
       <c r="F33" s="16">
-        <v>21.239380737813143</v>
+        <v>33.003964492164805</v>
       </c>
       <c r="G33" s="16">
-        <v>21.868453296842812</v>
+        <v>42.338833276680255</v>
       </c>
       <c r="H33" s="16">
-        <v>28.620908105782696</v>
+        <v>50.172706455002995</v>
       </c>
       <c r="I33" s="16">
-        <v>16.57176566926892</v>
+        <v>39.574780355782721</v>
       </c>
       <c r="J33" s="16">
-        <v>23.615399445075923</v>
+        <v>23.057182049490603</v>
       </c>
       <c r="K33" s="16">
-        <v>21.576153857674697</v>
+        <v>19.048344075891784</v>
       </c>
       <c r="L33" s="16">
-        <v>24.813850564692189</v>
+        <v>21.481514210162892</v>
       </c>
       <c r="M33" s="16">
-        <v>30.306456532698682</v>
+        <v>18.115850908998514</v>
       </c>
       <c r="N33" s="16">
-        <v>33.300588375307939</v>
+        <v>20.679702753300546</v>
       </c>
       <c r="O33" s="16">
-        <v>15.569903165791542</v>
+        <v>22.085933924873434</v>
       </c>
       <c r="P33" s="16">
-        <v>19.096514905237218</v>
-      </c>
-      <c r="Q33" s="31"/>
+        <v>13.290366478193151</v>
+      </c>
+      <c r="Q33" s="16">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="16">
-        <v>13.3231770085488</v>
+        <v>35.524400738676341</v>
       </c>
       <c r="E34" s="16">
-        <v>14.947408502944862</v>
+        <v>45.403420335985643</v>
       </c>
       <c r="F34" s="16">
-        <v>20.612282631289872</v>
+        <v>35.67372171666905</v>
       </c>
       <c r="G34" s="16">
-        <v>21.810233831843821</v>
+        <v>44.324841323157756</v>
       </c>
       <c r="H34" s="16">
-        <v>31.580794338047511</v>
+        <v>51.365667230180513</v>
       </c>
       <c r="I34" s="16">
-        <v>16.336951373050013</v>
+        <v>42.155403417412046</v>
       </c>
       <c r="J34" s="16">
-        <v>23.536874783143453</v>
+        <v>23.320678028402405</v>
       </c>
       <c r="K34" s="16">
-        <v>20.781078549530967</v>
+        <v>19.717988374234295</v>
       </c>
       <c r="L34" s="16">
-        <v>24.231370244694812</v>
+        <v>22.565254965961532</v>
       </c>
       <c r="M34" s="16">
-        <v>29.796795629524667</v>
+        <v>19.131642435267874</v>
       </c>
       <c r="N34" s="16">
-        <v>32.331249850946065</v>
+        <v>21.405379816313594</v>
       </c>
       <c r="O34" s="16">
-        <v>15.460808768934939</v>
+        <v>23.802663209890316</v>
       </c>
       <c r="P34" s="16">
-        <v>19.149801807626279</v>
-      </c>
-      <c r="Q34" s="31"/>
-    </row>
-    <row r="35" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13.968630674154097</v>
+      </c>
+      <c r="Q34" s="16">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
@@ -2359,99 +2408,103 @@
         <v>4</v>
       </c>
       <c r="D35" s="16">
-        <v>16.816017468582331</v>
+        <v>34.937966325921565</v>
       </c>
       <c r="E35" s="16">
-        <v>16.656432819748947</v>
+        <v>40.025342396149952</v>
       </c>
       <c r="F35" s="16">
-        <v>21.936013645292753</v>
+        <v>29.757564599462217</v>
       </c>
       <c r="G35" s="16">
-        <v>21.932251240884487</v>
+        <v>40.090317720015314</v>
       </c>
       <c r="H35" s="16">
-        <v>25.292385978318809</v>
+        <v>48.834976975707399</v>
       </c>
       <c r="I35" s="16">
-        <v>16.835987101956384</v>
+        <v>36.737399067049523</v>
       </c>
       <c r="J35" s="16">
-        <v>23.697958067349091</v>
+        <v>22.797195558030481</v>
       </c>
       <c r="K35" s="16">
-        <v>22.438096680686812</v>
+        <v>18.388950301669212</v>
       </c>
       <c r="L35" s="16">
-        <v>25.448531995394273</v>
+        <v>20.402520679941826</v>
       </c>
       <c r="M35" s="16">
-        <v>30.862157141656372</v>
+        <v>17.094741091820271</v>
       </c>
       <c r="N35" s="16">
-        <v>34.357577691815081</v>
+        <v>19.940922159102712</v>
       </c>
       <c r="O35" s="16">
-        <v>15.68880546767458</v>
+        <v>20.340711553536092</v>
       </c>
       <c r="P35" s="16">
-        <v>19.03737344064535</v>
-      </c>
-      <c r="Q35" s="31"/>
-    </row>
-    <row r="36" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>27</v>
+        <v>12.593673786232706</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="D36" s="16">
-        <v>5.0050408474612667</v>
+        <v>14.980993583120011</v>
       </c>
       <c r="E36" s="16">
-        <v>15.199877458936328</v>
+        <v>15.782630902499408</v>
       </c>
       <c r="F36" s="16">
-        <v>13.244358948423123</v>
+        <v>21.239380737813143</v>
       </c>
       <c r="G36" s="16">
-        <v>7.8936298235279043</v>
+        <v>21.868453296842812</v>
       </c>
       <c r="H36" s="16">
-        <v>18.412319077539543</v>
+        <v>28.620908105782696</v>
       </c>
       <c r="I36" s="16">
-        <v>21.39425343514112</v>
+        <v>16.57176566926892</v>
       </c>
       <c r="J36" s="16">
-        <v>20.37419545157174</v>
+        <v>23.615399445075923</v>
       </c>
       <c r="K36" s="16">
-        <v>17.559795089461929</v>
+        <v>21.576153857674697</v>
       </c>
       <c r="L36" s="16">
-        <v>23.54181329822454</v>
+        <v>24.813850564692189</v>
       </c>
       <c r="M36" s="16">
-        <v>9.7814403969714476</v>
+        <v>30.306456532698682</v>
       </c>
       <c r="N36" s="16">
-        <v>15.895976592336902</v>
+        <v>33.300588375307939</v>
       </c>
       <c r="O36" s="16">
-        <v>15.431849180748594</v>
+        <v>15.569903165791542</v>
       </c>
       <c r="P36" s="16">
-        <v>11.923173213098794</v>
-      </c>
-      <c r="Q36" s="31"/>
+        <v>19.096514905237218</v>
+      </c>
+      <c r="Q36" s="16">
+        <v>25.4</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -2461,45 +2514,47 @@
         <v>33</v>
       </c>
       <c r="D37" s="16">
-        <v>4.9910703183897471</v>
+        <v>13.3231770085488</v>
       </c>
       <c r="E37" s="16">
-        <v>14.580407995723835</v>
+        <v>14.947408502944862</v>
       </c>
       <c r="F37" s="16">
-        <v>12.694536401949772</v>
+        <v>20.612282631289872</v>
       </c>
       <c r="G37" s="16">
-        <v>7.3022704780706356</v>
+        <v>21.810233831843821</v>
       </c>
       <c r="H37" s="16">
-        <v>17.12627348202502</v>
+        <v>31.580794338047511</v>
       </c>
       <c r="I37" s="16">
-        <v>19.902241350915418</v>
+        <v>16.336951373050013</v>
       </c>
       <c r="J37" s="16">
-        <v>18.389801845083543</v>
+        <v>23.536874783143453</v>
       </c>
       <c r="K37" s="16">
-        <v>15.75684747748228</v>
+        <v>20.781078549530967</v>
       </c>
       <c r="L37" s="16">
-        <v>22.249203888313041</v>
+        <v>24.231370244694812</v>
       </c>
       <c r="M37" s="16">
-        <v>8.8993788797454574</v>
+        <v>29.796795629524667</v>
       </c>
       <c r="N37" s="16">
-        <v>14.320885005874089</v>
+        <v>32.331249850946065</v>
       </c>
       <c r="O37" s="16">
-        <v>14.746660640556426</v>
+        <v>15.460808768934939</v>
       </c>
       <c r="P37" s="16">
-        <v>10.945122024518023</v>
-      </c>
-      <c r="Q37" s="31"/>
+        <v>19.149801807626279</v>
+      </c>
+      <c r="Q37" s="16">
+        <v>24.3</v>
+      </c>
     </row>
     <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -2512,96 +2567,100 @@
         <v>4</v>
       </c>
       <c r="D38" s="16">
-        <v>5.0223457020442774</v>
+        <v>16.816017468582331</v>
       </c>
       <c r="E38" s="16">
-        <v>15.98971335888681</v>
+        <v>16.656432819748947</v>
       </c>
       <c r="F38" s="16">
-        <v>13.950362693192776</v>
+        <v>21.936013645292753</v>
       </c>
       <c r="G38" s="16">
-        <v>8.6542146318471769</v>
+        <v>21.932251240884487</v>
       </c>
       <c r="H38" s="16">
-        <v>20.038086648531461</v>
+        <v>25.292385978318809</v>
       </c>
       <c r="I38" s="16">
-        <v>23.294374049448368</v>
+        <v>16.835987101956384</v>
       </c>
       <c r="J38" s="16">
-        <v>22.845597238166345</v>
+        <v>23.697958067349091</v>
       </c>
       <c r="K38" s="16">
-        <v>19.854367582381908</v>
+        <v>22.438096680686812</v>
       </c>
       <c r="L38" s="16">
-        <v>25.206391335765652</v>
+        <v>25.448531995394273</v>
       </c>
       <c r="M38" s="16">
-        <v>10.893360919362737</v>
+        <v>30.862157141656372</v>
       </c>
       <c r="N38" s="16">
-        <v>17.858219329297828</v>
+        <v>34.357577691815081</v>
       </c>
       <c r="O38" s="16">
-        <v>16.325680533022233</v>
+        <v>15.68880546767458</v>
       </c>
       <c r="P38" s="16">
-        <v>13.205043717586292</v>
-      </c>
-      <c r="Q38" s="31"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>32</v>
+        <v>19.03737344064535</v>
+      </c>
+      <c r="Q38" s="16">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>29</v>
       </c>
       <c r="D39" s="16">
-        <v>0</v>
+        <v>5.0050408474612667</v>
       </c>
       <c r="E39" s="16">
-        <v>0</v>
+        <v>15.199877458936328</v>
       </c>
       <c r="F39" s="16">
-        <v>0</v>
+        <v>13.244358948423123</v>
       </c>
       <c r="G39" s="16">
-        <v>0</v>
+        <v>7.8936298235279043</v>
       </c>
       <c r="H39" s="16">
-        <v>0</v>
+        <v>18.412319077539543</v>
       </c>
       <c r="I39" s="16">
-        <v>0</v>
+        <v>21.39425343514112</v>
       </c>
       <c r="J39" s="16">
-        <v>40.875892692669147</v>
+        <v>20.37419545157174</v>
       </c>
       <c r="K39" s="16">
-        <v>33.42178613184317</v>
+        <v>17.559795089461929</v>
       </c>
       <c r="L39" s="16">
-        <v>38.278868442020823</v>
+        <v>23.54181329822454</v>
       </c>
       <c r="M39" s="16">
-        <v>24.59943985776184</v>
+        <v>9.7814403969714476</v>
       </c>
       <c r="N39" s="16">
-        <v>33.489020691882608</v>
+        <v>15.895976592336902</v>
       </c>
       <c r="O39" s="16">
-        <v>35.470047966126785</v>
+        <v>15.431849180748594</v>
       </c>
       <c r="P39" s="16">
-        <v>20.664792285937565</v>
-      </c>
-      <c r="Q39" s="31"/>
+        <v>11.923173213098794</v>
+      </c>
+      <c r="Q39" s="16">
+        <v>16.8</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2610,151 +2669,263 @@
       <c r="B40" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="16">
+        <v>4.9910703183897471</v>
+      </c>
+      <c r="E40" s="16">
+        <v>14.580407995723835</v>
+      </c>
+      <c r="F40" s="16">
+        <v>12.694536401949772</v>
+      </c>
+      <c r="G40" s="16">
+        <v>7.3022704780706356</v>
+      </c>
+      <c r="H40" s="16">
+        <v>17.12627348202502</v>
+      </c>
+      <c r="I40" s="16">
+        <v>19.902241350915418</v>
+      </c>
+      <c r="J40" s="16">
+        <v>18.389801845083543</v>
+      </c>
+      <c r="K40" s="16">
+        <v>15.75684747748228</v>
+      </c>
+      <c r="L40" s="16">
+        <v>22.249203888313041</v>
+      </c>
+      <c r="M40" s="16">
+        <v>8.8993788797454574</v>
+      </c>
+      <c r="N40" s="16">
+        <v>14.320885005874089</v>
+      </c>
+      <c r="O40" s="16">
+        <v>14.746660640556426</v>
+      </c>
+      <c r="P40" s="16">
+        <v>10.945122024518023</v>
+      </c>
+      <c r="Q40" s="16">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="16">
+        <v>5.0223457020442774</v>
+      </c>
+      <c r="E41" s="16">
+        <v>15.98971335888681</v>
+      </c>
+      <c r="F41" s="16">
+        <v>13.950362693192776</v>
+      </c>
+      <c r="G41" s="16">
+        <v>8.6542146318471769</v>
+      </c>
+      <c r="H41" s="16">
+        <v>20.038086648531461</v>
+      </c>
+      <c r="I41" s="16">
+        <v>23.294374049448368</v>
+      </c>
+      <c r="J41" s="16">
+        <v>22.845597238166345</v>
+      </c>
+      <c r="K41" s="16">
+        <v>19.854367582381908</v>
+      </c>
+      <c r="L41" s="16">
+        <v>25.206391335765652</v>
+      </c>
+      <c r="M41" s="16">
+        <v>10.893360919362737</v>
+      </c>
+      <c r="N41" s="16">
+        <v>17.858219329297828</v>
+      </c>
+      <c r="O41" s="16">
+        <v>16.325680533022233</v>
+      </c>
+      <c r="P41" s="16">
+        <v>13.205043717586292</v>
+      </c>
+      <c r="Q41" s="16">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="16">
         <v>0</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E42" s="16">
         <v>0</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F42" s="16">
         <v>0</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G42" s="16">
         <v>0</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H42" s="16">
         <v>0</v>
       </c>
-      <c r="I40" s="16">
+      <c r="I42" s="16">
         <v>0</v>
       </c>
-      <c r="J40" s="16">
+      <c r="J42" s="16">
+        <v>40.875892692669147</v>
+      </c>
+      <c r="K42" s="16">
+        <v>33.42178613184317</v>
+      </c>
+      <c r="L42" s="16">
+        <v>38.278868442020823</v>
+      </c>
+      <c r="M42" s="16">
+        <v>24.59943985776184</v>
+      </c>
+      <c r="N42" s="16">
+        <v>33.489020691882608</v>
+      </c>
+      <c r="O42" s="16">
+        <v>35.470047966126785</v>
+      </c>
+      <c r="P42" s="16">
+        <v>20.664792285937565</v>
+      </c>
+      <c r="Q42" s="16">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="16">
+        <v>0</v>
+      </c>
+      <c r="E43" s="16">
+        <v>0</v>
+      </c>
+      <c r="F43" s="16">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <v>0</v>
+      </c>
+      <c r="H43" s="16">
+        <v>0</v>
+      </c>
+      <c r="I43" s="16">
+        <v>0</v>
+      </c>
+      <c r="J43" s="16">
         <v>40.214976654346749</v>
       </c>
-      <c r="K40" s="16">
+      <c r="K43" s="16">
         <v>31.961883196169364</v>
       </c>
-      <c r="L40" s="16">
+      <c r="L43" s="16">
         <v>35.847234240268811</v>
       </c>
-      <c r="M40" s="16">
+      <c r="M43" s="16">
         <v>23.18714858505685</v>
       </c>
-      <c r="N40" s="16">
+      <c r="N43" s="16">
         <v>30.88827139481976</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O43" s="16">
         <v>33.896959570732115</v>
       </c>
-      <c r="P40" s="16">
+      <c r="P43" s="16">
         <v>19.658727502190441</v>
       </c>
-      <c r="Q40" s="31"/>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="Q43" s="16">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D44" s="17">
         <v>0</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E44" s="17">
         <v>0</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F44" s="17">
         <v>0</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G44" s="17">
         <v>0</v>
       </c>
-      <c r="H41" s="17">
+      <c r="H44" s="17">
         <v>0</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I44" s="17">
         <v>0</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J44" s="17">
         <v>41.620641890921341</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K44" s="17">
         <v>35.041317754766766</v>
       </c>
-      <c r="L41" s="17">
+      <c r="L44" s="17">
         <v>41.029123148407564</v>
       </c>
-      <c r="M41" s="17">
+      <c r="M44" s="17">
         <v>26.170218976651135</v>
       </c>
-      <c r="N41" s="17">
+      <c r="N44" s="17">
         <v>36.383303207045699</v>
       </c>
-      <c r="O41" s="17">
+      <c r="O44" s="17">
         <v>37.273729754326382</v>
       </c>
-      <c r="P41" s="17">
+      <c r="P44" s="17">
         <v>21.814125473305914</v>
       </c>
-      <c r="Q41" s="31"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
+      <c r="Q44" s="17">
+        <v>14.8</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -2773,6 +2944,57 @@
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
     </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="130" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ c82d120140ef1d00c878e859e656a9360e86e372 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.1.xlsx
+++ b/en/downloads/data-excel/1.2.1.xlsx
@@ -836,7 +836,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -920,6 +922,9 @@
       <c r="Q4" s="15">
         <v>2020</v>
       </c>
+      <c r="R4" s="15">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
@@ -972,6 +977,9 @@
       </c>
       <c r="Q5" s="25">
         <v>25.3</v>
+      </c>
+      <c r="R5" s="25">
+        <v>33.262233298138462</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -998,6 +1006,7 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1051,7 +1060,9 @@
       <c r="Q7" s="16">
         <v>25.3</v>
       </c>
-      <c r="R7" s="7"/>
+      <c r="R7" s="16">
+        <v>33.10733359588</v>
+      </c>
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1106,7 +1117,9 @@
       <c r="Q8" s="16">
         <v>25.3</v>
       </c>
-      <c r="R8" s="7"/>
+      <c r="R8" s="16">
+        <v>33.434791912906064</v>
+      </c>
       <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1133,7 +1146,7 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
-      <c r="R9" s="7"/>
+      <c r="R9" s="16"/>
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1176,7 +1189,9 @@
       <c r="Q10" s="16">
         <v>18.3</v>
       </c>
-      <c r="R10" s="7"/>
+      <c r="R10" s="16">
+        <v>33.257744153601877</v>
+      </c>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1219,7 +1234,9 @@
       <c r="Q11" s="16">
         <v>29.3</v>
       </c>
-      <c r="R11" s="7"/>
+      <c r="R11" s="16">
+        <v>33.264901349775037</v>
+      </c>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1246,7 +1263,7 @@
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
-      <c r="R12" s="7"/>
+      <c r="R12" s="16"/>
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1301,6 +1318,9 @@
       <c r="Q13" s="16">
         <v>31.8</v>
       </c>
+      <c r="R13" s="16">
+        <v>40.506761643955343</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1354,6 +1374,9 @@
       <c r="Q14" s="16">
         <v>22</v>
       </c>
+      <c r="R14" s="16">
+        <v>31.172874511993772</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1407,6 +1430,9 @@
       <c r="Q15" s="16">
         <v>21.7</v>
       </c>
+      <c r="R15" s="16">
+        <v>29.650854888195603</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1459,6 +1485,9 @@
       </c>
       <c r="Q16" s="16">
         <v>17.8</v>
+      </c>
+      <c r="R16" s="16">
+        <v>24.097659040517694</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,6 +1514,7 @@
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -1538,7 +1568,9 @@
       <c r="Q18" s="16">
         <v>34.700000000000003</v>
       </c>
-      <c r="R18" s="7"/>
+      <c r="R18" s="16">
+        <v>40.671537678982844</v>
+      </c>
       <c r="S18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1593,7 +1625,9 @@
       <c r="Q19" s="16">
         <v>34.299999999999997</v>
       </c>
-      <c r="R19" s="7"/>
+      <c r="R19" s="16">
+        <v>40.835744431591088</v>
+      </c>
       <c r="S19" s="7"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1648,7 +1682,9 @@
       <c r="Q20" s="16">
         <v>35.1</v>
       </c>
-      <c r="R20" s="7"/>
+      <c r="R20" s="16">
+        <v>40.494322790314847</v>
+      </c>
       <c r="S20" s="7"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1703,7 +1739,9 @@
       <c r="Q21" s="16">
         <v>37.200000000000003</v>
       </c>
-      <c r="R21" s="7"/>
+      <c r="R21" s="16">
+        <v>43.213901910043809</v>
+      </c>
       <c r="S21" s="7"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1758,7 +1796,9 @@
       <c r="Q22" s="16">
         <v>39</v>
       </c>
-      <c r="R22" s="7"/>
+      <c r="R22" s="16">
+        <v>43.25339669708363</v>
+      </c>
       <c r="S22" s="7"/>
     </row>
     <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1813,6 +1853,9 @@
       <c r="Q23" s="16">
         <v>35.4</v>
       </c>
+      <c r="R23" s="16">
+        <v>43.172054336673064</v>
+      </c>
     </row>
     <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
@@ -1866,6 +1909,9 @@
       <c r="Q24" s="16">
         <v>27.9</v>
       </c>
+      <c r="R24" s="16">
+        <v>38.130315382405762</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1919,6 +1965,9 @@
       <c r="Q25" s="16">
         <v>29</v>
       </c>
+      <c r="R25" s="16">
+        <v>39.052986923894757</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1972,6 +2021,9 @@
       <c r="Q26" s="16">
         <v>26.7</v>
       </c>
+      <c r="R26" s="16">
+        <v>37.162402419999459</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
@@ -2025,6 +2077,9 @@
       <c r="Q27" s="16">
         <v>36.799999999999997</v>
       </c>
+      <c r="R27" s="16">
+        <v>39.151777291250745</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -2078,6 +2133,9 @@
       <c r="Q28" s="16">
         <v>37.6</v>
       </c>
+      <c r="R28" s="16">
+        <v>39.257524172776719</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -2131,6 +2189,9 @@
       <c r="Q29" s="16">
         <v>35.9</v>
       </c>
+      <c r="R29" s="16">
+        <v>39.034895273433577</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
@@ -2184,6 +2245,9 @@
       <c r="Q30" s="16">
         <v>18.8</v>
       </c>
+      <c r="R30" s="16">
+        <v>23.758244663001044</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2237,6 +2301,9 @@
       <c r="Q31" s="16">
         <v>18.899999999999999</v>
       </c>
+      <c r="R31" s="16">
+        <v>23.600989554960133</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -2290,8 +2357,11 @@
       <c r="Q32" s="16">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="16">
+        <v>23.928051635532135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>21</v>
       </c>
@@ -2343,8 +2413,11 @@
       <c r="Q33" s="16">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="16">
+        <v>23.479873624436866</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
@@ -2396,8 +2469,11 @@
       <c r="Q34" s="16">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="16">
+        <v>24.191255182099319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
@@ -2449,8 +2525,11 @@
       <c r="Q35" s="16">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="16">
+        <v>22.759796314587014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>24</v>
       </c>
@@ -2502,8 +2581,11 @@
       <c r="Q36" s="16">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="16">
+        <v>27.00352039684709</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2555,8 +2637,11 @@
       <c r="Q37" s="16">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="16">
+        <v>26.49991066711625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -2608,8 +2693,11 @@
       <c r="Q38" s="16">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R38" s="16">
+        <v>27.572066513890491</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>27</v>
       </c>
@@ -2661,8 +2749,11 @@
       <c r="Q39" s="16">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="16">
+        <v>35.769118603355516</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
@@ -2714,8 +2805,11 @@
       <c r="Q40" s="16">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="16">
+        <v>35.037028356467729</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>2</v>
       </c>
@@ -2767,8 +2861,11 @@
       <c r="Q41" s="16">
         <v>17.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="16">
+        <v>36.714712776303102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>30</v>
       </c>
@@ -2820,8 +2917,11 @@
       <c r="Q42" s="16">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="16">
+        <v>28.585005142864613</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>35</v>
       </c>
@@ -2873,8 +2973,11 @@
       <c r="Q43" s="16">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="16">
+        <v>27.745516596290607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>2</v>
       </c>
@@ -2926,8 +3029,11 @@
       <c r="Q44" s="17">
         <v>14.8</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="17">
+        <v>29.549901683892372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -2944,7 +3050,7 @@
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ d0bca759f32cb3bb315e1f39e6e0ba8a25bbfc1f 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.1.xlsx
+++ b/en/downloads/data-excel/1.2.1.xlsx
@@ -418,7 +418,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -523,6 +523,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -837,7 +843,7 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,6 +931,9 @@
       <c r="R4" s="15">
         <v>2021</v>
       </c>
+      <c r="S4" s="15">
+        <v>2022</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
@@ -980,6 +989,9 @@
       </c>
       <c r="R5" s="25">
         <v>33.262233298138462</v>
+      </c>
+      <c r="S5" s="25">
+        <v>33.152856050161155</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1007,6 +1019,7 @@
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1063,7 +1076,9 @@
       <c r="R7" s="16">
         <v>33.10733359588</v>
       </c>
-      <c r="S7" s="7"/>
+      <c r="S7" s="37">
+        <v>32.831913512166025</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1120,7 +1135,9 @@
       <c r="R8" s="16">
         <v>33.434791912906064</v>
       </c>
-      <c r="S8" s="7"/>
+      <c r="S8" s="37">
+        <v>33.509346380994529</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
@@ -1147,7 +1164,6 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
-      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1192,7 +1208,9 @@
       <c r="R10" s="16">
         <v>33.257744153601877</v>
       </c>
-      <c r="S10" s="7"/>
+      <c r="S10" s="37">
+        <v>34.041194942162896</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1237,7 +1255,9 @@
       <c r="R11" s="16">
         <v>33.264901349775037</v>
       </c>
-      <c r="S11" s="7"/>
+      <c r="S11" s="37">
+        <v>32.636018013483323</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
@@ -1264,7 +1284,6 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
-      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1321,6 +1340,9 @@
       <c r="R13" s="16">
         <v>40.506761643955343</v>
       </c>
+      <c r="S13" s="37">
+        <v>40.271414365477746</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1377,6 +1399,9 @@
       <c r="R14" s="16">
         <v>31.172874511993772</v>
       </c>
+      <c r="S14" s="37">
+        <v>31.568157010024336</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1433,6 +1458,9 @@
       <c r="R15" s="16">
         <v>29.650854888195603</v>
       </c>
+      <c r="S15" s="37">
+        <v>30.277813022272248</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1488,6 +1516,9 @@
       </c>
       <c r="R16" s="16">
         <v>24.097659040517694</v>
+      </c>
+      <c r="S16" s="37">
+        <v>22.733608300917229</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1571,7 +1602,9 @@
       <c r="R18" s="16">
         <v>40.671537678982844</v>
       </c>
-      <c r="S18" s="7"/>
+      <c r="S18" s="37">
+        <v>48.492370829119814</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1628,7 +1661,9 @@
       <c r="R19" s="16">
         <v>40.835744431591088</v>
       </c>
-      <c r="S19" s="7"/>
+      <c r="S19" s="37">
+        <v>46.987664282528065</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1685,7 +1720,9 @@
       <c r="R20" s="16">
         <v>40.494322790314847</v>
       </c>
-      <c r="S20" s="7"/>
+      <c r="S20" s="37">
+        <v>50.118899291215271</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
@@ -1742,7 +1779,9 @@
       <c r="R21" s="16">
         <v>43.213901910043809</v>
       </c>
-      <c r="S21" s="7"/>
+      <c r="S21" s="37">
+        <v>47.142900749295329</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1799,7 +1838,9 @@
       <c r="R22" s="16">
         <v>43.25339669708363</v>
       </c>
-      <c r="S22" s="7"/>
+      <c r="S22" s="37">
+        <v>47.199946558584017</v>
+      </c>
     </row>
     <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
@@ -1856,6 +1897,9 @@
       <c r="R23" s="16">
         <v>43.172054336673064</v>
       </c>
+      <c r="S23" s="37">
+        <v>47.082025761639336</v>
+      </c>
     </row>
     <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
@@ -1912,6 +1956,9 @@
       <c r="R24" s="16">
         <v>38.130315382405762</v>
       </c>
+      <c r="S24" s="37">
+        <v>31.240016364696597</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1968,6 +2015,9 @@
       <c r="R25" s="16">
         <v>39.052986923894757</v>
       </c>
+      <c r="S25" s="37">
+        <v>31.228685777194666</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -2024,6 +2074,9 @@
       <c r="R26" s="16">
         <v>37.162402419999459</v>
       </c>
+      <c r="S26" s="37">
+        <v>31.252112297543153</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
@@ -2080,6 +2133,9 @@
       <c r="R27" s="16">
         <v>39.151777291250745</v>
       </c>
+      <c r="S27" s="37">
+        <v>42.049857693482664</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -2136,6 +2192,9 @@
       <c r="R28" s="16">
         <v>39.257524172776719</v>
       </c>
+      <c r="S28" s="37">
+        <v>42.689244289315013</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -2192,6 +2251,9 @@
       <c r="R29" s="16">
         <v>39.034895273433577</v>
       </c>
+      <c r="S29" s="37">
+        <v>41.380596558931735</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
@@ -2248,6 +2310,9 @@
       <c r="R30" s="16">
         <v>23.758244663001044</v>
       </c>
+      <c r="S30" s="37">
+        <v>19.945481087558658</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2304,6 +2369,9 @@
       <c r="R31" s="16">
         <v>23.600989554960133</v>
       </c>
+      <c r="S31" s="37">
+        <v>20.799187962023481</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -2360,8 +2428,11 @@
       <c r="R32" s="16">
         <v>23.928051635532135</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="37">
+        <v>19.013188474520234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>21</v>
       </c>
@@ -2416,8 +2487,11 @@
       <c r="R33" s="16">
         <v>23.479873624436866</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="37">
+        <v>23.919779113642239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
@@ -2472,8 +2546,11 @@
       <c r="R34" s="16">
         <v>24.191255182099319</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="37">
+        <v>23.962040711070269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
@@ -2528,8 +2605,11 @@
       <c r="R35" s="16">
         <v>22.759796314587014</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="37">
+        <v>23.876854008981983</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>24</v>
       </c>
@@ -2584,8 +2664,11 @@
       <c r="R36" s="16">
         <v>27.00352039684709</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="37">
+        <v>26.113584517813127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2640,8 +2723,11 @@
       <c r="R37" s="16">
         <v>26.49991066711625</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S37" s="37">
+        <v>25.651528441631889</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -2696,8 +2782,11 @@
       <c r="R38" s="16">
         <v>27.572066513890491</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S38" s="37">
+        <v>26.620973515499056</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>27</v>
       </c>
@@ -2752,8 +2841,11 @@
       <c r="R39" s="16">
         <v>35.769118603355516</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="37">
+        <v>35.676666099583812</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
@@ -2808,8 +2900,11 @@
       <c r="R40" s="16">
         <v>35.037028356467729</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S40" s="37">
+        <v>34.026766685280904</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>2</v>
       </c>
@@ -2864,8 +2959,11 @@
       <c r="R41" s="16">
         <v>36.714712776303102</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="37">
+        <v>37.792274390474752</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>30</v>
       </c>
@@ -2920,8 +3018,11 @@
       <c r="R42" s="16">
         <v>28.585005142864613</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="37">
+        <v>26.602385500795538</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>35</v>
       </c>
@@ -2976,8 +3077,11 @@
       <c r="R43" s="16">
         <v>27.745516596290607</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S43" s="37">
+        <v>25.585637135242425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>2</v>
       </c>
@@ -3032,8 +3136,11 @@
       <c r="R44" s="17">
         <v>29.549901683892372</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="38">
+        <v>27.750206810614948</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3050,7 +3157,7 @@
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ fa727193d3653d1e75f6d95b559963a078b26bde 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.1.xlsx
+++ b/en/downloads/data-excel/1.2.1.xlsx
@@ -840,11 +840,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -853,7 +851,7 @@
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>43</v>
       </c>
@@ -864,7 +862,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>41</v>
       </c>
@@ -875,8 +873,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -934,8 +932,11 @@
       <c r="S4" s="15">
         <v>2022</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="15">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>5</v>
       </c>
@@ -993,8 +994,11 @@
       <c r="S5" s="25">
         <v>33.152856050161155</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="25">
+        <v>29.810232786618478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>64</v>
       </c>
@@ -1020,8 +1024,9 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="25"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1079,8 +1084,11 @@
       <c r="S7" s="37">
         <v>32.831913512166025</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="37">
+        <v>29.669466599025686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -1138,8 +1146,11 @@
       <c r="S8" s="37">
         <v>33.509346380994529</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="37">
+        <v>29.964546620904322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>67</v>
       </c>
@@ -1165,7 +1176,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
@@ -1175,15 +1186,27 @@
       <c r="C10" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="D10" s="16">
+        <v>23.2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>22.6</v>
+      </c>
+      <c r="F10" s="16">
+        <v>21.9</v>
+      </c>
       <c r="G10" s="16">
         <v>23.6</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="H10" s="16">
+        <v>30.7</v>
+      </c>
+      <c r="I10" s="16">
+        <v>35.4</v>
+      </c>
+      <c r="J10" s="16">
+        <v>28.5</v>
+      </c>
       <c r="K10" s="16">
         <v>26.9</v>
       </c>
@@ -1211,8 +1234,11 @@
       <c r="S10" s="37">
         <v>34.041194942162896</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="37">
+        <v>30.196132774743152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -1222,15 +1248,27 @@
       <c r="C11" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="D11" s="16">
+        <v>41.7</v>
+      </c>
+      <c r="E11" s="16">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F11" s="16">
+        <v>37.1</v>
+      </c>
       <c r="G11" s="16">
         <v>39.5</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="H11" s="16">
+        <v>40.4</v>
+      </c>
+      <c r="I11" s="16">
+        <v>39.6</v>
+      </c>
+      <c r="J11" s="16">
+        <v>41.4</v>
+      </c>
       <c r="K11" s="16">
         <v>32.6</v>
       </c>
@@ -1258,8 +1296,11 @@
       <c r="S11" s="37">
         <v>32.636018013483323</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="37">
+        <v>29.586576623908091</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>61</v>
       </c>
@@ -1285,7 +1326,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -1343,8 +1384,11 @@
       <c r="S13" s="37">
         <v>40.271414365477746</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="37">
+        <v>36.679314997357302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
@@ -1402,8 +1446,11 @@
       <c r="S14" s="37">
         <v>31.568157010024336</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T14" s="37">
+        <v>27.761651579699627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>56</v>
       </c>
@@ -1461,8 +1508,11 @@
       <c r="S15" s="37">
         <v>30.277813022272248</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T15" s="37">
+        <v>26.945499612171261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1520,8 +1570,11 @@
       <c r="S16" s="37">
         <v>22.733608300917229</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T16" s="37">
+        <v>19.920707357966336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>58</v>
       </c>
@@ -1547,7 +1600,7 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>8</v>
       </c>
@@ -1605,8 +1658,11 @@
       <c r="S18" s="37">
         <v>48.492370829119814</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="37">
+        <v>48.132487638243802</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
@@ -1664,8 +1720,11 @@
       <c r="S19" s="37">
         <v>46.987664282528065</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="37">
+        <v>47.095468608697217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -1723,8 +1782,11 @@
       <c r="S20" s="37">
         <v>50.118899291215271</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="37">
+        <v>49.224436679851941</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>11</v>
       </c>
@@ -1782,8 +1844,11 @@
       <c r="S21" s="37">
         <v>47.142900749295329</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="37">
+        <v>36.060409324309092</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
@@ -1841,8 +1906,11 @@
       <c r="S22" s="37">
         <v>47.199946558584017</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T22" s="37">
+        <v>36.438841751655779</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>2</v>
       </c>
@@ -1900,8 +1968,11 @@
       <c r="S23" s="37">
         <v>47.082025761639336</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T23" s="37">
+        <v>35.670056408825062</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>13</v>
       </c>
@@ -1959,8 +2030,11 @@
       <c r="S24" s="37">
         <v>31.240016364696597</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="37">
+        <v>30.852411825788565</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
@@ -2018,8 +2092,11 @@
       <c r="S25" s="37">
         <v>31.228685777194666</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="37">
+        <v>30.330534800771165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
@@ -2077,8 +2154,11 @@
       <c r="S26" s="37">
         <v>31.252112297543153</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="37">
+        <v>31.403214482728419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>15</v>
       </c>
@@ -2136,8 +2216,11 @@
       <c r="S27" s="37">
         <v>42.049857693482664</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="37">
+        <v>38.094443042646382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
@@ -2195,8 +2278,11 @@
       <c r="S28" s="37">
         <v>42.689244289315013</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="37">
+        <v>38.158675127516169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2254,8 +2340,11 @@
       <c r="S29" s="37">
         <v>41.380596558931735</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="37">
+        <v>38.024712001344874</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>18</v>
       </c>
@@ -2313,8 +2402,11 @@
       <c r="S30" s="37">
         <v>19.945481087558658</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="37">
+        <v>20.396452079475392</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
@@ -2372,8 +2464,11 @@
       <c r="S31" s="37">
         <v>20.799187962023481</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="37">
+        <v>20.655435559889604</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -2431,8 +2526,11 @@
       <c r="S32" s="37">
         <v>19.013188474520234</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="37">
+        <v>20.117912106064367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>21</v>
       </c>
@@ -2490,8 +2588,11 @@
       <c r="S33" s="37">
         <v>23.919779113642239</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="37">
+        <v>23.188885535955222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
@@ -2549,8 +2650,11 @@
       <c r="S34" s="37">
         <v>23.962040711070269</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="37">
+        <v>23.078628487453106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
@@ -2608,8 +2712,11 @@
       <c r="S35" s="37">
         <v>23.876854008981983</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35" s="37">
+        <v>23.300729383023359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>24</v>
       </c>
@@ -2667,8 +2774,11 @@
       <c r="S36" s="37">
         <v>26.113584517813127</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="37">
+        <v>26.600808028614065</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2726,8 +2836,11 @@
       <c r="S37" s="37">
         <v>25.651528441631889</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T37" s="37">
+        <v>26.440501693813694</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -2785,8 +2898,11 @@
       <c r="S38" s="37">
         <v>26.620973515499056</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T38" s="37">
+        <v>26.779307280034676</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>27</v>
       </c>
@@ -2844,8 +2960,11 @@
       <c r="S39" s="37">
         <v>35.676666099583812</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39" s="37">
+        <v>32.389629740110649</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
@@ -2903,8 +3022,11 @@
       <c r="S40" s="37">
         <v>34.026766685280904</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T40" s="37">
+        <v>31.71205247152805</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>2</v>
       </c>
@@ -2962,8 +3084,11 @@
       <c r="S41" s="37">
         <v>37.792274390474752</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T41" s="37">
+        <v>33.231499210635427</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>30</v>
       </c>
@@ -3021,8 +3146,11 @@
       <c r="S42" s="37">
         <v>26.602385500795538</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T42" s="37">
+        <v>13.872134221368512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>35</v>
       </c>
@@ -3080,8 +3208,11 @@
       <c r="S43" s="37">
         <v>25.585637135242425</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T43" s="37">
+        <v>14.562707317462859</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>2</v>
       </c>
@@ -3139,8 +3270,11 @@
       <c r="S44" s="38">
         <v>27.750206810614948</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="38">
+        <v>13.080583219648313</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3157,7 +3291,7 @@
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>

</xml_diff>